<commit_message>
Todos arquivos gerado ajustando todos alunos +18
</commit_message>
<xml_diff>
--- a/data/depara.xlsx
+++ b/data/depara.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renato.vinicius\Documents\Python\Trabalho Pratico PUC\projeto_integracao\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21B1B4E-8A42-42D1-89A8-E68FA53B3CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21ABFBF6-1BFF-459A-B115-D31D79427AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alunos" sheetId="6" r:id="rId1"/>
@@ -867,7 +867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -892,9 +892,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4214,8 +4211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34878EAA-DC9A-492A-9624-C4538CF74757}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4241,7 +4238,7 @@
       <c r="D1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>227</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -11477,7 +11474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338E5FE9-7681-424E-9D10-559E2F8269C4}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>